<commit_message>
MDT combined all interfaces into a single file
</commit_message>
<xml_diff>
--- a/MDT/DienstenCatalogus/ProcVerloop.xlsx
+++ b/MDT/DienstenCatalogus/ProcVerloop.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Selectie BBS.PROC-VERLOOP'!$A$1:$O$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1339,7 +1339,7 @@
   <dimension ref="A1:O1544"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
MDT WIP producten samenhang weer op orde gemaakt
</commit_message>
<xml_diff>
--- a/MDT/DienstenCatalogus/ProcVerloop.xlsx
+++ b/MDT/DienstenCatalogus/ProcVerloop.xlsx
@@ -489,16 +489,7 @@
     <t>Foutbericht</t>
   </si>
   <si>
-    <t>ProcIdVerloop</t>
-  </si>
-  <si>
     <t>[ProcIdVerloop]</t>
-  </si>
-  <si>
-    <t>procID</t>
-  </si>
-  <si>
-    <t>ProcID</t>
   </si>
   <si>
     <t>VolgNummer</t>
@@ -517,6 +508,15 @@
   </si>
   <si>
     <t>volgNummer</t>
+  </si>
+  <si>
+    <t>ProcIdent</t>
+  </si>
+  <si>
+    <t>procIdent</t>
+  </si>
+  <si>
+    <t>ProcVerloop</t>
   </si>
 </sst>
 </file>
@@ -1339,7 +1339,7 @@
   <dimension ref="A1:O1544"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1387,36 +1387,36 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="D2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="M2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="D3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" t="s">
+        <v>157</v>
+      </c>
+      <c r="M3" t="s">
         <v>159</v>
-      </c>
-      <c r="F3" t="s">
-        <v>160</v>
-      </c>
-      <c r="M3" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>